<commit_message>
adding middleware for authentication
</commit_message>
<xml_diff>
--- a/files/individual.xlsx
+++ b/files/individual.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Description</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>puri bhaji</t>
+    <t>pav bhaji</t>
   </si>
 </sst>
 </file>
@@ -410,14 +410,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
       <c r="B3">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -425,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>